<commit_message>
Updated Run30 Channel_Map and Run_Parameters to versions which include simulation sheets
</commit_message>
<xml_diff>
--- a/config/30th/Run_Parameters_Run30.xlsx
+++ b/config/30th/Run_Parameters_Run30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Documents\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B864C-D9D7-4970-B799-3CA6118E97D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF503C1-E1F2-471F-894C-6938DB489884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1305" windowWidth="21600" windowHeight="11385" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200911_OvernightBi207_AfterFi" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="20200922_Afternoon_AfterFifthIn" sheetId="7" r:id="rId8"/>
     <sheet name="20200923_Afternoon_AfterSixthIn" sheetId="8" r:id="rId9"/>
     <sheet name="20200924_Afternoon_AfterSeventh" sheetId="10" r:id="rId10"/>
+    <sheet name="simulations" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -451,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A59307-BDC9-4EC8-9E53-61962D86FD2C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -538,6 +539,112 @@
       </c>
       <c r="B10" s="2">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978291A6-2C18-4ECD-9213-C2A54449AF9E}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added 20200916_Morning_Noise to RunParameters and ChannelMap for Run30
</commit_message>
<xml_diff>
--- a/config/30th/Run_Parameters_Run30.xlsx
+++ b/config/30th/Run_Parameters_Run30.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlenardo/Research/Software/StanfordTPCAnalysis/config/30th/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF503C1-E1F2-471F-894C-6938DB489884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263C777F-2980-F149-BE81-69E30ED8B945}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1305" windowWidth="21600" windowHeight="11385" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1300" windowWidth="26400" windowHeight="18760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200911_OvernightBi207_AfterFi" sheetId="1" r:id="rId1"/>
     <sheet name="20200912_MorningNoise_PreRecirc" sheetId="3" r:id="rId2"/>
     <sheet name="20200915_Night_AfterFirstRnInje" sheetId="2" r:id="rId3"/>
-    <sheet name="20200916_RnPoAlphaEffTest" sheetId="4" r:id="rId4"/>
-    <sheet name="20200917_Night_AfterThirdRnInje" sheetId="5" r:id="rId5"/>
-    <sheet name="20200920_Rn220InParallel_RnPoTe" sheetId="9" r:id="rId6"/>
-    <sheet name="20200921_Afternoon_AfterFourthI" sheetId="6" r:id="rId7"/>
-    <sheet name="20200922_Afternoon_AfterFifthIn" sheetId="7" r:id="rId8"/>
-    <sheet name="20200923_Afternoon_AfterSixthIn" sheetId="8" r:id="rId9"/>
-    <sheet name="20200924_Afternoon_AfterSeventh" sheetId="10" r:id="rId10"/>
-    <sheet name="20201207_alpha_sim" sheetId="11" r:id="rId11"/>
+    <sheet name="20200916_Morning_Noise" sheetId="12" r:id="rId4"/>
+    <sheet name="20200916_RnPoAlphaEffTest" sheetId="4" r:id="rId5"/>
+    <sheet name="20200917_Night_AfterThirdRnInje" sheetId="5" r:id="rId6"/>
+    <sheet name="20200920_Rn220InParallel_RnPoTe" sheetId="9" r:id="rId7"/>
+    <sheet name="20200921_Afternoon_AfterFourthI" sheetId="6" r:id="rId8"/>
+    <sheet name="20200922_Afternoon_AfterFifthIn" sheetId="7" r:id="rId9"/>
+    <sheet name="20200923_Afternoon_AfterSixthIn" sheetId="8" r:id="rId10"/>
+    <sheet name="20200924_Afternoon_AfterSeventh" sheetId="10" r:id="rId11"/>
+    <sheet name="20201207_alpha_sim" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -350,12 +351,12 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -363,7 +364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -371,7 +372,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -379,7 +380,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -387,7 +388,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -395,7 +396,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -403,7 +404,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -411,7 +412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -419,7 +420,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -427,7 +428,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -435,7 +436,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -449,6 +450,112 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD57A0D-B95F-4502-BB57-4E7E0AAB34F5}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A59307-BDC9-4EC8-9E53-61962D86FD2C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -456,12 +563,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -477,7 +584,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -485,7 +592,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -493,7 +600,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -501,7 +608,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -509,7 +616,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -517,7 +624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -525,7 +632,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -533,7 +640,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -541,7 +648,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -554,20 +661,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978291A6-2C18-4ECD-9213-C2A54449AF9E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -583,7 +690,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -591,7 +698,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -599,7 +706,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -607,7 +714,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -615,7 +722,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -623,7 +730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -631,7 +738,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -639,7 +746,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -647,7 +754,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -668,13 +775,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -690,7 +797,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -698,7 +805,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -706,7 +813,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -714,7 +821,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -722,7 +829,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -730,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -738,7 +845,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -746,7 +853,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -754,7 +861,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -778,12 +885,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -799,7 +906,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -807,7 +914,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -815,7 +922,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -823,7 +930,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -831,7 +938,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -839,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -847,7 +954,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -855,7 +962,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -863,7 +970,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -877,6 +984,115 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DEF9E3-758B-C344-8D95-496C7FD0B0A2}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D085C840-42CC-4CF7-9CF8-CBE18E3603A8}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -884,12 +1100,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,7 +1113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -905,7 +1121,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -913,7 +1129,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -921,7 +1137,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -929,7 +1145,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -937,7 +1153,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -945,7 +1161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -953,7 +1169,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -961,7 +1177,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -969,7 +1185,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -982,7 +1198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4F2E08-EA34-4243-B491-9C13C1A3CF3C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -990,12 +1206,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1011,7 +1227,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1235,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1243,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1035,7 +1251,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1043,7 +1259,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1275,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1067,7 +1283,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1075,7 +1291,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1088,7 +1304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A3A6E7-0AB7-42C8-A30D-B3095917031C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1096,12 +1312,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1333,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1341,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1349,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1141,7 +1357,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1365,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1157,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1381,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1173,7 +1389,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1397,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF636D12-5059-4999-9A9A-6C34B6516DC9}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1202,12 +1418,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1215,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1223,7 +1439,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1231,7 +1447,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1239,7 +1455,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1463,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1255,7 +1471,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1263,7 +1479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1271,7 +1487,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1279,7 +1495,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1287,7 +1503,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1300,7 +1516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604252A7-6ACC-415E-931D-94C9B9BDB3B7}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1308,12 +1524,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1329,7 +1545,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1553,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1345,7 +1561,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1569,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1361,7 +1577,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1369,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1593,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1601,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1393,113 +1609,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD57A0D-B95F-4502-BB57-4E7E0AAB34F5}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>7.8125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Changes to allow propagation of MC truth values, and first attempt at Cole's noise reduction (although it doesn't work
</commit_message>
<xml_diff>
--- a/config/30th/Run_Parameters_Run30.xlsx
+++ b/config/30th/Run_Parameters_Run30.xlsx
@@ -1,30 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlenardo/Research/Software/StanfordTPCAnalysis/config/30th/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263C777F-2980-F149-BE81-69E30ED8B945}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF503C1-E1F2-471F-894C-6938DB489884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1300" windowWidth="26400" windowHeight="18760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="1305" windowWidth="21600" windowHeight="11385" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20200911_OvernightBi207_AfterFi" sheetId="1" r:id="rId1"/>
     <sheet name="20200912_MorningNoise_PreRecirc" sheetId="3" r:id="rId2"/>
     <sheet name="20200915_Night_AfterFirstRnInje" sheetId="2" r:id="rId3"/>
-    <sheet name="20200916_Morning_Noise" sheetId="12" r:id="rId4"/>
-    <sheet name="20200916_RnPoAlphaEffTest" sheetId="4" r:id="rId5"/>
-    <sheet name="20200917_Night_AfterThirdRnInje" sheetId="5" r:id="rId6"/>
-    <sheet name="20200920_Rn220InParallel_RnPoTe" sheetId="9" r:id="rId7"/>
-    <sheet name="20200921_Afternoon_AfterFourthI" sheetId="6" r:id="rId8"/>
-    <sheet name="20200922_Afternoon_AfterFifthIn" sheetId="7" r:id="rId9"/>
-    <sheet name="20200923_Afternoon_AfterSixthIn" sheetId="8" r:id="rId10"/>
-    <sheet name="20200924_Afternoon_AfterSeventh" sheetId="10" r:id="rId11"/>
-    <sheet name="20201207_alpha_sim" sheetId="11" r:id="rId12"/>
+    <sheet name="20200916_RnPoAlphaEffTest" sheetId="4" r:id="rId4"/>
+    <sheet name="20200917_Night_AfterThirdRnInje" sheetId="5" r:id="rId5"/>
+    <sheet name="20200920_Rn220InParallel_RnPoTe" sheetId="9" r:id="rId6"/>
+    <sheet name="20200921_Afternoon_AfterFourthI" sheetId="6" r:id="rId7"/>
+    <sheet name="20200922_Afternoon_AfterFifthIn" sheetId="7" r:id="rId8"/>
+    <sheet name="20200923_Afternoon_AfterSixthIn" sheetId="8" r:id="rId9"/>
+    <sheet name="20200924_Afternoon_AfterSeventh" sheetId="10" r:id="rId10"/>
+    <sheet name="simulations" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -351,12 +350,12 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -364,7 +363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -372,7 +371,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -380,7 +379,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -388,7 +387,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -396,7 +395,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -404,7 +403,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -412,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -420,7 +419,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -428,7 +427,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -436,7 +435,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -450,112 +449,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD57A0D-B95F-4502-BB57-4E7E0AAB34F5}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>7.8125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A59307-BDC9-4EC8-9E53-61962D86FD2C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -563,12 +456,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -584,7 +477,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -592,7 +485,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -600,7 +493,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -608,7 +501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -616,7 +509,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -624,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -632,7 +525,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -640,7 +533,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -648,7 +541,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -661,20 +554,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978291A6-2C18-4ECD-9213-C2A54449AF9E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -690,7 +583,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -698,7 +591,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -706,7 +599,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -714,7 +607,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -722,7 +615,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -730,7 +623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -738,7 +631,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -746,7 +639,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -754,7 +647,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -775,13 +668,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -797,7 +690,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -805,7 +698,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,7 +706,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -821,7 +714,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -829,7 +722,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -837,7 +730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,7 +738,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -853,7 +746,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -861,7 +754,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -885,12 +778,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -898,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -906,7 +799,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -914,7 +807,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -922,7 +815,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -930,7 +823,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -938,7 +831,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -946,7 +839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -954,7 +847,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -962,7 +855,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -970,7 +863,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -984,115 +877,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DEF9E3-758B-C344-8D95-496C7FD0B0A2}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>62.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>7.8125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>11.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D085C840-42CC-4CF7-9CF8-CBE18E3603A8}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1100,12 +884,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1121,7 +905,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +913,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +921,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +929,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +937,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +953,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +961,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +969,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4F2E08-EA34-4243-B491-9C13C1A3CF3C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1206,12 +990,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1011,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1235,7 +1019,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1027,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1251,7 +1035,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1043,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1267,7 +1051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1275,7 +1059,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1283,7 +1067,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1291,7 +1075,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1304,7 +1088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A3A6E7-0AB7-42C8-A30D-B3095917031C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1312,12 +1096,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1333,7 +1117,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1125,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1133,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1357,7 +1141,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1365,7 +1149,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1373,7 +1157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1165,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1173,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1397,7 +1181,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1410,7 +1194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF636D12-5059-4999-9A9A-6C34B6516DC9}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1418,12 +1202,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1439,7 +1223,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1447,7 +1231,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1455,7 +1239,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1463,7 +1247,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1471,7 +1255,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1487,7 +1271,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1495,7 +1279,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1287,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1516,7 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{604252A7-6ACC-415E-931D-94C9B9BDB3B7}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1524,12 +1308,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1329,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1553,7 +1337,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1345,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1569,7 +1353,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1577,7 +1361,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1593,7 +1377,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1601,7 +1385,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1393,113 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD57A0D-B95F-4502-BB57-4E7E0AAB34F5}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>